<commit_message>
Reworking setup to work from a central access program that calls the rest as needed.
</commit_message>
<xml_diff>
--- a/The new organizer.xlsx
+++ b/The new organizer.xlsx
@@ -5,6 +5,7 @@
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Big sheet 1" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Big sheet 2" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -3534,4 +3535,22 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>